<commit_message>
misc updates: addition of postUni function in utils and portBounce script to shut/noshut ACI Node interface
</commit_message>
<xml_diff>
--- a/partool/values.xlsx
+++ b/partool/values.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="720" windowWidth="36280" windowHeight="23280" activeTab="1"/>
+    <workbookView xWindow="2120" yWindow="720" windowWidth="36280" windowHeight="23280"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="57">
   <si>
     <t>vpcId</t>
   </si>
@@ -156,24 +156,6 @@
     <t>p2:0101:leaf01:leaf02:port1:vpc</t>
   </si>
   <si>
-    <t>sea0305-0101-leaf01</t>
-  </si>
-  <si>
-    <t>sea0305-0101-leaf02</t>
-  </si>
-  <si>
-    <t>sea0305-0101-leaf01:02:vpc</t>
-  </si>
-  <si>
-    <t>sea0305-0102-leaf01:02:vpc</t>
-  </si>
-  <si>
-    <t>sea0305-0102-leaf01</t>
-  </si>
-  <si>
-    <t>sea0305-0102-leaf02</t>
-  </si>
-  <si>
     <t>p2:0101:leaf01:leaf02:port2:vpc</t>
   </si>
   <si>
@@ -202,6 +184,21 @@
   </si>
   <si>
     <t>tenant</t>
+  </si>
+  <si>
+    <t>leaf01</t>
+  </si>
+  <si>
+    <t>leaf02</t>
+  </si>
+  <si>
+    <t>leaf01:02:vpc</t>
+  </si>
+  <si>
+    <t>leaf01:leaf02:port1:vpc</t>
+  </si>
+  <si>
+    <t>leaf01:leaf02:port2:vpc</t>
   </si>
 </sst>
 </file>
@@ -556,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,10 +582,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>201</v>
@@ -599,10 +596,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <v>202</v>
@@ -613,10 +610,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>203</v>
@@ -627,10 +624,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C5">
         <v>204</v>
@@ -648,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,66 +665,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -780,7 +777,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
@@ -803,7 +800,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
@@ -818,7 +815,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>34</v>
@@ -826,7 +823,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -841,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>34</v>
@@ -849,7 +846,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>36</v>
@@ -864,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>34</v>
@@ -881,7 +878,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -936,7 +933,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -971,7 +968,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -1006,7 +1003,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -1041,7 +1038,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>19</v>
@@ -1091,32 +1088,32 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>